<commit_message>
Planning and High Level System
Planning and High Level System /Mahesh Prasath
</commit_message>
<xml_diff>
--- a/Calyxtract/SourceCode/branch/MaheshPrasath/Planing.xlsx
+++ b/Calyxtract/SourceCode/branch/MaheshPrasath/Planing.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Board Bring Up" sheetId="1" r:id="rId1"/>
+    <sheet name="Slave Module" sheetId="2" r:id="rId2"/>
+    <sheet name="Master Board" sheetId="3" r:id="rId3"/>
+    <sheet name="System Architecture" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
   <si>
     <t>S No</t>
   </si>
@@ -211,13 +214,293 @@
   </si>
   <si>
     <t>Khaleel/Sunil/Mahesh (GUI)</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Sub Modules</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Board Type</t>
+  </si>
+  <si>
+    <t>Slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera </t>
+  </si>
+  <si>
+    <t>To be implemente in 16 Bit
+Need to consult Anupam for clarification</t>
+  </si>
+  <si>
+    <t>Camera Initi ( hw.h) (Hw C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camer Image Processing (IMF.h) (Camera FilterClass)
+1. Gray Scale Converstion
+2. Gaussian Filter 
+3. Sober Filter </t>
+  </si>
+  <si>
+    <t>1. Orentation Detection (Detection.h) ( Detction Class)
+2. Pod Detection
+3. Quality Detection</t>
+  </si>
+  <si>
+    <t>CAN initi ( hw.h) (Hw C)</t>
+  </si>
+  <si>
+    <t>CAN Parser
+1. Packer Encode
+2. Packe Decode</t>
+  </si>
+  <si>
+    <t>Transmitter 
+Receiver 
+Error Check</t>
+  </si>
+  <si>
+    <t>Make Priority is set as a parameter</t>
+  </si>
+  <si>
+    <t>VFD Drive Control</t>
+  </si>
+  <si>
+    <t>Modbus Initi (Modbus.h ) Mobus Class</t>
+  </si>
+  <si>
+    <t>Jonson Parser</t>
+  </si>
+  <si>
+    <t>RS232.h ( Hw.h)</t>
+  </si>
+  <si>
+    <t>Commands ( Fw, Rv, Stp, Speed) Motor.h Motor class</t>
+  </si>
+  <si>
+    <t>Modbus to RS232 protocol Converter Modbus.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Encoder</t>
+  </si>
+  <si>
+    <t>Initi Endcoder Pins (Hw.h) hardware Class</t>
+  </si>
+  <si>
+    <t>QEI function ( encoder.h) Dr, Speed)</t>
+  </si>
+  <si>
+    <t>GPIO init ( hw.h) hardware class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penamatic </t>
+  </si>
+  <si>
+    <t>Send Penamatic  name and Status</t>
+  </si>
+  <si>
+    <t>ONOFF (Penamatic .h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sensor</t>
+  </si>
+  <si>
+    <t>Return Senosor Name and Status</t>
+  </si>
+  <si>
+    <t>Read Status (Sensor Name) Sensor.h Sensor Class</t>
+  </si>
+  <si>
+    <t>Error Indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Coler pattern </t>
+  </si>
+  <si>
+    <t>Parmater Error Status</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>ADC init, Hw.h hw Class</t>
+  </si>
+  <si>
+    <t>Read ADC</t>
+  </si>
+  <si>
+    <t>Data Conversion</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>Flash Memory Init, Hw.h Hw Class</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>Sector and Block wise operation</t>
+  </si>
+  <si>
+    <t>Erase</t>
+  </si>
+  <si>
+    <t>Error Check Read ID, etc</t>
+  </si>
+  <si>
+    <t>Read  FLashNu.h FlashNu Class</t>
+  </si>
+  <si>
+    <t>UART inti hw.h hw class</t>
+  </si>
+  <si>
+    <t>Protocol Encode</t>
+  </si>
+  <si>
+    <t>Protocol Decode</t>
+  </si>
+  <si>
+    <t>Read  UARTNum.h UARTNu class</t>
+  </si>
+  <si>
+    <t>Two UASRTs</t>
+  </si>
+  <si>
+    <t>Name the use case</t>
+  </si>
+  <si>
+    <t>Application Layer</t>
+  </si>
+  <si>
+    <t>Call the respective function for Camera</t>
+  </si>
+  <si>
+    <t>Call the Calculations for Pematic operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call the function stepper Motor drive  </t>
+  </si>
+  <si>
+    <t>Stepper Motor</t>
+  </si>
+  <si>
+    <t>ONOFF (Stepper .h)</t>
+  </si>
+  <si>
+    <t>Speed Control</t>
+  </si>
+  <si>
+    <t>Direction Control</t>
+  </si>
+  <si>
+    <t>Commminicate with Master board</t>
+  </si>
+  <si>
+    <t>read Encoder parameters</t>
+  </si>
+  <si>
+    <t>Check Sensor Status</t>
+  </si>
+  <si>
+    <t>Check for Switch configuration ( Jumper or Sw Flags)</t>
+  </si>
+  <si>
+    <t>Remote Firm Update ( OTA)</t>
+  </si>
+  <si>
+    <t>Commincation to Master/Slave (CAN)</t>
+  </si>
+  <si>
+    <t>Send command</t>
+  </si>
+  <si>
+    <t>Receive Command</t>
+  </si>
+  <si>
+    <t>Parase Command</t>
+  </si>
+  <si>
+    <t>Formate command</t>
+  </si>
+  <si>
+    <t>function to take address to send and the data</t>
+  </si>
+  <si>
+    <t>Team Member</t>
+  </si>
+  <si>
+    <t>Elevator Control</t>
+  </si>
+  <si>
+    <t>GPIO Init (Modbus)</t>
+  </si>
+  <si>
+    <t>ON OFF</t>
+  </si>
+  <si>
+    <t>Sensor Input</t>
+  </si>
+  <si>
+    <t>Speed Monitor Encoder</t>
+  </si>
+  <si>
+    <t>Vibration Sensor</t>
+  </si>
+  <si>
+    <t>Or 1</t>
+  </si>
+  <si>
+    <t>Channle 1</t>
+  </si>
+  <si>
+    <t>Channle 2</t>
+  </si>
+  <si>
+    <t>Channle 3</t>
+  </si>
+  <si>
+    <t>Or 2</t>
+  </si>
+  <si>
+    <t>Or 3</t>
+  </si>
+  <si>
+    <t>33 Kgs / hr</t>
+  </si>
+  <si>
+    <t>Raspebrry Pi</t>
+  </si>
+  <si>
+    <t>Mater Board (Elevator and Slave corodnation with cloud)</t>
+  </si>
+  <si>
+    <t>Pod 1, pod 2, Pod 3</t>
+  </si>
+  <si>
+    <t>Pod 1, Pod 2, Pod3</t>
+  </si>
+  <si>
+    <t>Pod 1, Pod 2, Pod 3</t>
+  </si>
+  <si>
+    <t>Q 1, Q 2, Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,16 +516,64 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -265,11 +596,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -279,6 +715,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,21 +1061,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -576,7 +1086,7 @@
     <col min="8" max="8" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -602,7 +1112,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -620,7 +1130,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -636,7 +1146,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -652,7 +1162,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -668,7 +1178,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -684,7 +1194,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -700,7 +1210,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -716,7 +1226,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -732,7 +1242,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
@@ -748,7 +1258,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -764,7 +1274,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -780,7 +1290,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -790,7 +1300,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -812,7 +1322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -826,7 +1336,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -840,7 +1350,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -854,7 +1364,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -864,7 +1374,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="30">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -886,7 +1396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -896,7 +1406,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="30">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -918,7 +1428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -928,7 +1438,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -950,7 +1460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -960,7 +1470,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -982,7 +1492,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -992,7 +1502,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>7</v>
       </c>
@@ -1021,4 +1531,1035 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="12"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>8</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>9</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>10</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="7">
+        <v>11</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="5">
+        <v>12</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
+        <v>13</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="24"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="24"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="24"/>
+      <c r="G50" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D39:D46"/>
+    <mergeCell ref="F47:F50"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="C3:C50"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>3</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C3:C24"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="D20:D24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D5:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>